<commit_message>
User input validation + usage of collections
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anishkoppisetty/Desktop/Framework/BankingAppDemo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C2B462-5C1A-A046-BDFC-58F51A819312}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F60DD5B1-EC4E-714B-B997-0A754A561B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -107,7 +107,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -476,108 +475,110 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.1640625"/>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+    <col min="8" max="8" width="37.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="0">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="0">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="0">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="0">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="0">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="0">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="0">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="0">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="0">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="G2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" t="s" s="0">
+      <c r="H2" t="s">
         <v>17</v>
       </c>
-      <c r="I2" t="s" s="0">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="n" s="0">
+      <c r="J2">
         <v>66.41</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s" s="0">
+      <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s" s="0">
+      <c r="F3" t="s">
         <v>23</v>
       </c>
-      <c r="G3" t="s" s="0">
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" t="n" s="0">
-        <v>50.0</v>
+      <c r="J3">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Transfer from Excel DB to JSON files for user details
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anishkoppisetty/Desktop/Framework/BankingAppDemo/"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
   <si>
     <t>Username</t>
   </si>
@@ -101,12 +101,31 @@
   </si>
   <si>
     <t>4695253629</t>
+  </si>
+  <si>
+    <t>jsonTestv1</t>
+  </si>
+  <si>
+    <t>testone</t>
+  </si>
+  <si>
+    <t>TT09182006</t>
+  </si>
+  <si>
+    <t>jsonTestv1@gmail.com</t>
+  </si>
+  <si>
+    <t>test st., Testv1, texas, US - 67676</t>
+  </si>
+  <si>
+    <t>1234567890</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -472,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
@@ -480,105 +499,137 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="8" max="8" width="37.83203125" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.1640625"/>
+    <col min="8" max="8" customWidth="true" width="37.83203125"/>
+    <col min="9" max="9" customWidth="true" width="15.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" t="s" s="0">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="0">
         <v>66.41</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>23</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="0">
         <v>50</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="J4" t="n" s="0">
+        <v>69.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>